<commit_message>
[IMP] z0bug-odoo: minor improvements
</commit_message>
<xml_diff>
--- a/z0bug_odoo/build/lib/z0bug_odoo/data/account_payment_term_line.xlsx
+++ b/z0bug_odoo/build/lib/z0bug_odoo/data/account_payment_term_line.xlsx
@@ -79,7 +79,7 @@
     <t xml:space="preserve">z0bug.payment_1</t>
   </si>
   <si>
-    <t xml:space="preserve">fix_day_following_month</t>
+    <t xml:space="preserve">after_invoice_month</t>
   </si>
   <si>
     <t xml:space="preserve">account_banking_riba.riba</t>
@@ -246,7 +246,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I8" activeCellId="0" sqref="I8"/>
+      <selection pane="topLeft" activeCell="I9" activeCellId="0" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>